<commit_message>
update after paris major
</commit_message>
<xml_diff>
--- a/core_df_main.xlsx
+++ b/core_df_main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>FS</t>
   </si>
@@ -34,66 +34,75 @@
     <t>Naive-</t>
   </si>
   <si>
+    <t>Gabbi</t>
+  </si>
+  <si>
+    <t>Miracle-</t>
+  </si>
+  <si>
+    <t>NeverEnd</t>
+  </si>
+  <si>
+    <t>Paparazi灬</t>
+  </si>
+  <si>
+    <t>Madara</t>
+  </si>
+  <si>
+    <t>Timado</t>
+  </si>
+  <si>
     <t>Ameame</t>
   </si>
   <si>
-    <t>Gabbi</t>
-  </si>
-  <si>
-    <t>NeverEnd</t>
+    <t>Ace</t>
+  </si>
+  <si>
+    <t>rtz</t>
+  </si>
+  <si>
+    <t>Fervian</t>
+  </si>
+  <si>
+    <t>RAMZeS666</t>
+  </si>
+  <si>
+    <t>Daxak</t>
   </si>
   <si>
     <t>DJ</t>
   </si>
   <si>
-    <t>Paparazi灬</t>
-  </si>
-  <si>
-    <t>Madara</t>
-  </si>
-  <si>
-    <t>Timado</t>
-  </si>
-  <si>
-    <t>rtz</t>
-  </si>
-  <si>
-    <t>Fervian</t>
-  </si>
-  <si>
-    <t>Daxak</t>
-  </si>
-  <si>
-    <t>RAMZeS666</t>
-  </si>
-  <si>
     <t>Aventador</t>
   </si>
   <si>
-    <t>Ace</t>
+    <t>Nisha</t>
+  </si>
+  <si>
+    <t>Monet</t>
+  </si>
+  <si>
+    <t>Frost</t>
+  </si>
+  <si>
+    <t>YawaR</t>
   </si>
   <si>
     <t>AhJit</t>
   </si>
   <si>
-    <t>Nisha</t>
-  </si>
-  <si>
-    <t>Monet</t>
-  </si>
-  <si>
-    <t>Frost</t>
-  </si>
-  <si>
-    <t>YawaR</t>
-  </si>
-  <si>
     <t>Taiga</t>
   </si>
   <si>
     <t>Kuku^</t>
   </si>
   <si>
+    <t>ana</t>
+  </si>
+  <si>
+    <t>hFn k3</t>
+  </si>
+  <si>
     <t>Sammyboy</t>
   </si>
   <si>
@@ -106,63 +115,69 @@
     <t>Moo</t>
   </si>
   <si>
+    <t>leo</t>
+  </si>
+  <si>
+    <t>Lelis</t>
+  </si>
+  <si>
     <t>MSS-</t>
   </si>
   <si>
-    <t>Miracle-</t>
-  </si>
-  <si>
     <t>eGo</t>
   </si>
   <si>
-    <t>hFn k3</t>
-  </si>
-  <si>
     <t>xiao8</t>
   </si>
   <si>
     <t>Jonassomfan</t>
   </si>
   <si>
+    <t>Faith_bian</t>
+  </si>
+  <si>
+    <t>Srf</t>
+  </si>
+  <si>
+    <t>dream`</t>
+  </si>
+  <si>
+    <t>ragingpotato</t>
+  </si>
+  <si>
+    <t>AtuunN</t>
+  </si>
+  <si>
+    <t>MinD_ContRoL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k1 el cacha viejas de 26 </t>
+  </si>
+  <si>
+    <t>Sneyking</t>
+  </si>
+  <si>
     <t>old eLeVeN</t>
   </si>
   <si>
-    <t>Faith_bian</t>
-  </si>
-  <si>
-    <t>Srf</t>
-  </si>
-  <si>
-    <t>AtuunN</t>
-  </si>
-  <si>
-    <t>MinD_ContRoL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k1 el cacha viejas de 26 </t>
+    <t>Kōtarō</t>
+  </si>
+  <si>
+    <t>iLTW</t>
+  </si>
+  <si>
+    <t>old chicken</t>
+  </si>
+  <si>
+    <t>Crystallize</t>
+  </si>
+  <si>
+    <t>Sylar</t>
   </si>
   <si>
     <t>Ceb</t>
   </si>
   <si>
-    <t>Sneyking</t>
-  </si>
-  <si>
-    <t>Kōtarō</t>
-  </si>
-  <si>
-    <t>iLTW</t>
-  </si>
-  <si>
-    <t>Crystallize</t>
-  </si>
-  <si>
-    <t>old chicken</t>
-  </si>
-  <si>
-    <t>Sylar</t>
-  </si>
-  <si>
     <t>Boxi</t>
   </si>
   <si>
@@ -184,49 +199,58 @@
     <t>Illidan Stormrage SF46</t>
   </si>
   <si>
+    <t>zai</t>
+  </si>
+  <si>
     <t>Fbz</t>
   </si>
   <si>
+    <t>Brax</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
     <t>iceiceice</t>
   </si>
   <si>
-    <t>zai</t>
-  </si>
-  <si>
     <t>4dr &lt;3 Déia</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
     <t>Yang</t>
   </si>
   <si>
     <t>s4</t>
   </si>
   <si>
+    <t>9pasha</t>
+  </si>
+  <si>
     <t>MoonMeander</t>
   </si>
   <si>
-    <t>9pasha</t>
-  </si>
-  <si>
     <t>Flyby</t>
   </si>
   <si>
+    <t>EternaLEnVy</t>
+  </si>
+  <si>
+    <t>Meracle-</t>
+  </si>
+  <si>
     <t>Universe</t>
   </si>
   <si>
     <t>633</t>
   </si>
   <si>
-    <t>EternaLEnVy</t>
+    <t>Zfreek</t>
   </si>
   <si>
     <t>KheZu</t>
   </si>
   <si>
-    <t>Brax</t>
+    <t>Chalice</t>
   </si>
   <si>
     <t>ryOyr</t>
@@ -235,9 +259,6 @@
     <t>Blizzy</t>
   </si>
   <si>
-    <t>Chalice</t>
-  </si>
-  <si>
     <t>Xxs</t>
   </si>
   <si>
@@ -253,6 +274,9 @@
     <t>kpii</t>
   </si>
   <si>
+    <t>monkeys-forever</t>
+  </si>
+  <si>
     <t>Ghostik</t>
   </si>
   <si>
@@ -262,9 +286,6 @@
     <t>p4pita</t>
   </si>
   <si>
-    <t>monkeys-forever</t>
-  </si>
-  <si>
     <t>Sword</t>
   </si>
   <si>
@@ -272,6 +293,9 @@
   </si>
   <si>
     <t>Emperor Crimson</t>
+  </si>
+  <si>
+    <t>Maden</t>
   </si>
 </sst>
 </file>
@@ -629,7 +653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -688,16 +712,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>452.3151689384472</v>
+        <v>288.0262813151182</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E4">
-        <v>12.5643102482902</v>
+        <v>12.52288179630949</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -705,16 +729,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>288.0262813151182</v>
+        <v>424.0105213662207</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E5">
-        <v>12.52288179630949</v>
+        <v>12.47089768724179</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -739,16 +763,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>160.6150802359194</v>
+        <v>856.051285616898</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="E7">
-        <v>12.3550061719938</v>
+        <v>12.2293040802414</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -756,16 +780,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>708.8157171452984</v>
+        <v>315.6385532479056</v>
       </c>
       <c r="C8">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E8">
-        <v>12.22096064043618</v>
+        <v>12.13994435568868</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -773,16 +797,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>315.6385532479056</v>
+        <v>157.7683442559032</v>
       </c>
       <c r="C9">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E9">
-        <v>12.13994435568868</v>
+        <v>12.13602648122332</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -790,16 +814,16 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>157.7683442559032</v>
+        <v>664.2857081277617</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D10">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="E10">
-        <v>12.13602648122332</v>
+        <v>12.0779219659593</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -807,16 +831,16 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>624.1686910024108</v>
+        <v>925.1532538951501</v>
       </c>
       <c r="C11">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D11">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E11">
-        <v>12.00324405773867</v>
+        <v>12.01497732331364</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -824,16 +848,16 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>321.4586821704658</v>
+        <v>804.4747036426703</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D12">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E12">
-        <v>11.90587711742466</v>
+        <v>12.00708512899508</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -841,16 +865,16 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>353.2703637927382</v>
+        <v>321.4586821704658</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D13">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E13">
-        <v>11.77567879309127</v>
+        <v>11.90587711742466</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -858,16 +882,16 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>762.0722063724243</v>
+        <v>898.7483612833597</v>
       </c>
       <c r="C14">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D14">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="E14">
-        <v>11.72418779034499</v>
+        <v>11.82563633267578</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -875,16 +899,16 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>127.4236085029072</v>
+        <v>353.2703637927382</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E15">
-        <v>11.5839644093552</v>
+        <v>11.77567879309127</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -892,16 +916,16 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>706.0392600308365</v>
+        <v>220.1934478657715</v>
       </c>
       <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
         <v>19</v>
       </c>
-      <c r="D16">
-        <v>61</v>
-      </c>
       <c r="E16">
-        <v>11.57441409886617</v>
+        <v>11.58912883504061</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -909,16 +933,16 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>148.144892673634</v>
+        <v>127.4236085029072</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D17">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>11.39576097489492</v>
+        <v>11.5839644093552</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -994,16 +1018,16 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>177.9257483819466</v>
+        <v>232.8226033776347</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E22">
-        <v>10.46622049305568</v>
+        <v>10.5828456080743</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1011,16 +1035,16 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>132.5163055758223</v>
+        <v>177.9257483819466</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E23">
-        <v>10.19356196737094</v>
+        <v>10.46622049305568</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1028,16 +1052,16 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>111.7395034792367</v>
+        <v>132.5163055758223</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E24">
-        <v>10.15813667993061</v>
+        <v>10.19356196737094</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1045,16 +1069,16 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>446.4427232219886</v>
+        <v>132.2032199440249</v>
       </c>
       <c r="C25">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E25">
-        <v>10.14642552777247</v>
+        <v>10.16947845723268</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1062,16 +1086,16 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>157.9659711064792</v>
+        <v>254.2037452718926</v>
       </c>
       <c r="C26">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D26">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E26">
-        <v>9.87287319415495</v>
+        <v>10.1681498108757</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1079,16 +1103,16 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>246.3852730341438</v>
+        <v>111.7395034792367</v>
       </c>
       <c r="C27">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E27">
-        <v>9.855410921365753</v>
+        <v>10.15813667993061</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1096,16 +1120,16 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>193.9817850221353</v>
+        <v>494.8251304946193</v>
       </c>
       <c r="C28">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D28">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E28">
-        <v>9.699089251106766</v>
+        <v>9.896502609892385</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1113,16 +1137,16 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>67.5861733650213</v>
+        <v>157.9659711064792</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E29">
-        <v>9.655167623574471</v>
+        <v>9.87287319415495</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1130,16 +1154,16 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>259.8519215234844</v>
+        <v>246.3852730341438</v>
       </c>
       <c r="C30">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D30">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E30">
-        <v>9.624145241610531</v>
+        <v>9.855410921365753</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1147,16 +1171,16 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>163.5857669330896</v>
+        <v>68.44819430654003</v>
       </c>
       <c r="C31">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E31">
-        <v>9.622692172534684</v>
+        <v>9.778313472362862</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1164,16 +1188,16 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>182.4121537428708</v>
+        <v>68.22041036100032</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E32">
-        <v>9.60063967067741</v>
+        <v>9.745772908714331</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1181,16 +1205,16 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>105.5416412973084</v>
+        <v>193.9817850221353</v>
       </c>
       <c r="C33">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D33">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E33">
-        <v>9.594694663391671</v>
+        <v>9.699089251106766</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1198,16 +1222,16 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>271.5008636958767</v>
+        <v>259.8519215234844</v>
       </c>
       <c r="C34">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D34">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E34">
-        <v>9.362098748133677</v>
+        <v>9.624145241610531</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1215,16 +1239,16 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>252.4224220011774</v>
+        <v>182.4121537428708</v>
       </c>
       <c r="C35">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E35">
-        <v>9.348978592636202</v>
+        <v>9.60063967067741</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1232,16 +1256,16 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>158.0832284456081</v>
+        <v>105.5416412973084</v>
       </c>
       <c r="C36">
         <v>8</v>
       </c>
       <c r="D36">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E36">
-        <v>9.299013437976946</v>
+        <v>9.594694663391671</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1249,16 +1273,16 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>74.18478648615219</v>
+        <v>252.4224220011774</v>
       </c>
       <c r="C37">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D37">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E37">
-        <v>9.273098310769024</v>
+        <v>9.348978592636202</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1266,16 +1290,16 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>306.0703318526064</v>
+        <v>158.0832284456081</v>
       </c>
       <c r="C38">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D38">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E38">
-        <v>9.002068583900188</v>
+        <v>9.299013437976946</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1283,16 +1307,16 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>125.6626670461858</v>
+        <v>46.49453602727273</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
       <c r="D39">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E39">
-        <v>8.975904789013274</v>
+        <v>9.298907205454546</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1300,16 +1324,16 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>169.6514339698798</v>
+        <v>83.48394992933807</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E40">
-        <v>8.929022840519989</v>
+        <v>9.275994436593118</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1317,16 +1341,16 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>285.6439411043024</v>
+        <v>74.18478648615219</v>
       </c>
       <c r="C41">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D41">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E41">
-        <v>8.926373159509449</v>
+        <v>9.273098310769024</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1334,16 +1358,16 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>97.88190464185192</v>
+        <v>551.334044534686</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D42">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E42">
-        <v>8.898354967441083</v>
+        <v>9.038263025158786</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1351,16 +1375,16 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>167.0211611590026</v>
+        <v>125.6626670461858</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E43">
-        <v>8.790587429421192</v>
+        <v>8.975904789013274</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1368,16 +1392,16 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>253.4598738681667</v>
+        <v>285.6439411043024</v>
       </c>
       <c r="C44">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D44">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E44">
-        <v>8.739995650626438</v>
+        <v>8.926373159509449</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1385,16 +1409,16 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>251.0431868210592</v>
+        <v>348.1155125362211</v>
       </c>
       <c r="C45">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D45">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E45">
-        <v>8.656661614519281</v>
+        <v>8.926038782980028</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1402,16 +1426,16 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>129.6874898055781</v>
+        <v>97.88190464185192</v>
       </c>
       <c r="C46">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D46">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E46">
-        <v>8.645832653705206</v>
+        <v>8.898354967441083</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1419,16 +1443,16 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>327.8448199716431</v>
+        <v>167.0211611590026</v>
       </c>
       <c r="C47">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D47">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E47">
-        <v>8.62749526241166</v>
+        <v>8.790587429421192</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1436,16 +1460,16 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>228.0949555921628</v>
+        <v>341.8477307262588</v>
       </c>
       <c r="C48">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D48">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E48">
-        <v>8.44796131822825</v>
+        <v>8.76532642887843</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1453,16 +1477,16 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>177.2778835861681</v>
+        <v>253.4598738681667</v>
       </c>
       <c r="C49">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D49">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E49">
-        <v>8.44180398029372</v>
+        <v>8.739995650626438</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1470,16 +1494,16 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>67.3453603997669</v>
+        <v>129.6874898055781</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D50">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E50">
-        <v>8.418170049970863</v>
+        <v>8.645832653705206</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1487,16 +1511,16 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>50.41828850872657</v>
+        <v>276.6206767388324</v>
       </c>
       <c r="C51">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E51">
-        <v>8.403048084787761</v>
+        <v>8.644396148088513</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1504,16 +1528,16 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>372.6635369038106</v>
+        <v>327.8448199716431</v>
       </c>
       <c r="C52">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D52">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E52">
-        <v>8.281411931195791</v>
+        <v>8.62749526241166</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1521,16 +1545,16 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>91.00638164752633</v>
+        <v>228.0949555921628</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D53">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E53">
-        <v>8.273307422502393</v>
+        <v>8.44796131822825</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1538,16 +1562,16 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>221.7811357484096</v>
+        <v>177.2778835861681</v>
       </c>
       <c r="C54">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D54">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E54">
-        <v>8.214116138829985</v>
+        <v>8.44180398029372</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1555,16 +1579,16 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>356.6510298666807</v>
+        <v>67.3453603997669</v>
       </c>
       <c r="C55">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D55">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="E55">
-        <v>8.105705224242742</v>
+        <v>8.418170049970863</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1572,16 +1596,16 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>420.1110433025078</v>
+        <v>50.41828850872657</v>
       </c>
       <c r="C56">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D56">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="E56">
-        <v>8.079058525048227</v>
+        <v>8.403048084787761</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1589,16 +1613,16 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>63.2277336760373</v>
+        <v>372.6635369038106</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D57">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E57">
-        <v>7.903466709504663</v>
+        <v>8.281411931195791</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1606,16 +1630,16 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>350.3486294665078</v>
+        <v>91.00638164752633</v>
       </c>
       <c r="C58">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D58">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E58">
-        <v>7.785525099255728</v>
+        <v>8.273307422502393</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1623,16 +1647,16 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>448.5969632358012</v>
+        <v>562.3338457387722</v>
       </c>
       <c r="C59">
         <v>36</v>
       </c>
       <c r="D59">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E59">
-        <v>7.734430400617262</v>
+        <v>8.269615378511356</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1640,16 +1664,16 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>400.6674070856699</v>
+        <v>221.7811357484096</v>
       </c>
       <c r="C60">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="D60">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="E60">
-        <v>7.70514244395519</v>
+        <v>8.214116138829985</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1657,16 +1681,16 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>179.5424263148689</v>
+        <v>138.6365073966063</v>
       </c>
       <c r="C61">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D61">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E61">
-        <v>7.480934429786206</v>
+        <v>8.155088670388604</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1674,16 +1698,16 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>484.3401184924101</v>
+        <v>492.6819760829945</v>
       </c>
       <c r="C62">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D62">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E62">
-        <v>7.45138643834477</v>
+        <v>8.076753706278598</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1691,16 +1715,16 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>81.88403934092456</v>
+        <v>400.0240811203193</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D63">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E63">
-        <v>7.444003576447687</v>
+        <v>8.000481622406387</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1708,16 +1732,16 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>151.3629226028161</v>
+        <v>63.2277336760373</v>
       </c>
       <c r="C64">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D64">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E64">
-        <v>7.207758219181717</v>
+        <v>7.903466709504663</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1725,16 +1749,16 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>79.24091788493672</v>
+        <v>544.8295837797173</v>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D65">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E65">
-        <v>7.20371980772152</v>
+        <v>7.783279768281675</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1742,16 +1766,16 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>56.51260960245819</v>
+        <v>517.7947916443532</v>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D66">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="E66">
-        <v>7.064076200307274</v>
+        <v>7.728280472303778</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1759,16 +1783,16 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>62.41805832888364</v>
+        <v>572.923959452571</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D67">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="E67">
-        <v>6.935339814320404</v>
+        <v>7.538473150691724</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1776,16 +1800,16 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>76.16145571581315</v>
+        <v>179.5424263148689</v>
       </c>
       <c r="C68">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D68">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E68">
-        <v>6.923768701437559</v>
+        <v>7.480934429786206</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1793,16 +1817,16 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>68.59118605417173</v>
+        <v>81.88403934092456</v>
       </c>
       <c r="C69">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D69">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E69">
-        <v>6.859118605417173</v>
+        <v>7.444003576447687</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1810,16 +1834,16 @@
         <v>72</v>
       </c>
       <c r="B70">
-        <v>197.247581161647</v>
+        <v>103.0498593549707</v>
       </c>
       <c r="C70">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D70">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E70">
-        <v>6.801640729711965</v>
+        <v>7.360704239640765</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1827,16 +1851,16 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>240.0959753270282</v>
+        <v>72.12612962897586</v>
       </c>
       <c r="C71">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D71">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E71">
-        <v>6.669332647973007</v>
+        <v>7.212612962897586</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1844,16 +1868,16 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>98.44853152452143</v>
+        <v>151.3629226028161</v>
       </c>
       <c r="C72">
         <v>25</v>
       </c>
       <c r="D72">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E72">
-        <v>6.563235434968095</v>
+        <v>7.207758219181717</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1861,16 +1885,16 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>58.83337113666917</v>
+        <v>79.24091788493672</v>
       </c>
       <c r="C73">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D73">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E73">
-        <v>6.537041237407686</v>
+        <v>7.20371980772152</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1878,16 +1902,16 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>51.3286148705429</v>
+        <v>71.72562486949394</v>
       </c>
       <c r="C74">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D74">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E74">
-        <v>6.416076858817862</v>
+        <v>7.172562486949394</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1895,16 +1919,16 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>160.0548321090597</v>
+        <v>62.41805832888364</v>
       </c>
       <c r="C75">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D75">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E75">
-        <v>6.402193284362388</v>
+        <v>6.935339814320404</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1912,16 +1936,16 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>82.38149690599911</v>
+        <v>381.4251390056971</v>
       </c>
       <c r="C76">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D76">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="E76">
-        <v>6.337038223538394</v>
+        <v>6.935002527376311</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1929,16 +1953,16 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>48.32542992241702</v>
+        <v>68.59118605417173</v>
       </c>
       <c r="C77">
         <v>20</v>
       </c>
       <c r="D77">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E77">
-        <v>6.040678740302128</v>
+        <v>6.859118605417173</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1946,16 +1970,16 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>48.06556469468836</v>
+        <v>197.247581161647</v>
       </c>
       <c r="C78">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D78">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E78">
-        <v>6.008195586836045</v>
+        <v>6.801640729711965</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1963,101 +1987,237 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>47.64972118807601</v>
+        <v>98.44853152452143</v>
       </c>
       <c r="C79">
+        <v>25</v>
+      </c>
+      <c r="D79">
+        <v>15</v>
+      </c>
+      <c r="E79">
+        <v>6.563235434968095</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80">
+        <v>58.83337113666917</v>
+      </c>
+      <c r="C80">
         <v>8</v>
       </c>
-      <c r="D79">
-        <v>8</v>
-      </c>
-      <c r="E79">
-        <v>5.956215148509502</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="1">
-        <v>117960951</v>
-      </c>
-      <c r="B80">
-        <v>29.74027187909091</v>
-      </c>
-      <c r="C80">
-        <v>3</v>
-      </c>
       <c r="D80">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E80">
-        <v>5.948054375818182</v>
+        <v>6.537041237407686</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B81">
-        <v>35.25262055413704</v>
+        <v>51.3286148705429</v>
       </c>
       <c r="C81">
+        <v>20</v>
+      </c>
+      <c r="D81">
         <v>8</v>
       </c>
-      <c r="D81">
-        <v>6</v>
-      </c>
       <c r="E81">
-        <v>5.87543675902284</v>
+        <v>6.416076858817862</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B82">
-        <v>71.73233922347546</v>
+        <v>160.0548321090597</v>
       </c>
       <c r="C82">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D82">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E82">
-        <v>5.517872247959651</v>
+        <v>6.402193284362388</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B83">
-        <v>135.0572889888193</v>
+        <v>138.6682349437776</v>
       </c>
       <c r="C83">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D83">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E83">
-        <v>5.194511114954588</v>
+        <v>6.303101588353527</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B84">
+        <v>96.86289718794032</v>
+      </c>
+      <c r="C84">
+        <v>11</v>
+      </c>
+      <c r="D84">
+        <v>16</v>
+      </c>
+      <c r="E84">
+        <v>6.05393107424627</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85">
+        <v>48.32542992241702</v>
+      </c>
+      <c r="C85">
+        <v>20</v>
+      </c>
+      <c r="D85">
+        <v>8</v>
+      </c>
+      <c r="E85">
+        <v>6.040678740302128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86">
+        <v>48.06556469468836</v>
+      </c>
+      <c r="C86">
+        <v>8</v>
+      </c>
+      <c r="D86">
+        <v>8</v>
+      </c>
+      <c r="E86">
+        <v>6.008195586836045</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B87">
+        <v>47.64972118807601</v>
+      </c>
+      <c r="C87">
+        <v>8</v>
+      </c>
+      <c r="D87">
+        <v>8</v>
+      </c>
+      <c r="E87">
+        <v>5.956215148509502</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="1">
+        <v>117960951</v>
+      </c>
+      <c r="B88">
+        <v>29.74027187909091</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <v>5</v>
+      </c>
+      <c r="E88">
+        <v>5.948054375818182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89">
+        <v>71.73233922347546</v>
+      </c>
+      <c r="C89">
+        <v>6</v>
+      </c>
+      <c r="D89">
+        <v>13</v>
+      </c>
+      <c r="E89">
+        <v>5.517872247959651</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90">
+        <v>181.5097995575433</v>
+      </c>
+      <c r="C90">
+        <v>36</v>
+      </c>
+      <c r="D90">
+        <v>34</v>
+      </c>
+      <c r="E90">
+        <v>5.338523516398332</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91">
         <v>10.35013405797102</v>
       </c>
-      <c r="C84">
+      <c r="C91">
         <v>3</v>
       </c>
-      <c r="D84">
+      <c r="D91">
         <v>2</v>
       </c>
-      <c r="E84">
+      <c r="E91">
         <v>5.175067028985508</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92">
+        <v>23.53091794863636</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+      <c r="D92">
+        <v>5</v>
+      </c>
+      <c r="E92">
+        <v>4.706183589727273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>